<commit_message>
Calculate Client security hash updated with SPA integration
</commit_message>
<xml_diff>
--- a/Final_Report.xlsx
+++ b/Final_Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kharkuzhali\Documents\UiPath\Client Security Hash Integration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPathProject\ACME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DC9822-6ECE-405B-B4BC-D334128DF88C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62853378-A431-4B37-87C2-E97D2AD4DB13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
   <si>
     <t>Actions</t>
   </si>
@@ -154,15 +154,9 @@
     <t>OZ56329</t>
   </si>
   <si>
-    <t>COMPLETED</t>
-  </si>
-  <si>
     <t>8a6b096afca2f039f0e9f61188f80de67f2476e2</t>
   </si>
   <si>
-    <t>HashKeyGenerated Successfully</t>
-  </si>
-  <si>
     <t>40dc24d603fd311b6ba3bfd09d814cf4da1ff979</t>
   </si>
   <si>
@@ -191,6 +185,9 @@
   </si>
   <si>
     <t>085d0662804652ab8f4e4b02961794739fc0114d</t>
+  </si>
+  <si>
+    <t>success</t>
   </si>
 </sst>
 </file>
@@ -559,7 +556,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +613,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -625,11 +622,9 @@
         <v>33</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
@@ -643,7 +638,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>14</v>
@@ -652,11 +647,9 @@
         <v>34</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -670,7 +663,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>16</v>
@@ -679,11 +672,9 @@
         <v>35</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
@@ -697,7 +688,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>18</v>
@@ -706,11 +697,9 @@
         <v>36</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -724,7 +713,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>20</v>
@@ -733,11 +722,9 @@
         <v>37</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -751,7 +738,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>22</v>
@@ -760,11 +747,9 @@
         <v>38</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -778,7 +763,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>24</v>
@@ -787,11 +772,9 @@
         <v>39</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -805,7 +788,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>26</v>
@@ -814,11 +797,9 @@
         <v>40</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -832,7 +813,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>28</v>
@@ -841,11 +822,9 @@
         <v>41</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
@@ -859,7 +838,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>30</v>
@@ -868,11 +847,9 @@
         <v>42</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -886,7 +863,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>32</v>
@@ -895,11 +872,9 @@
         <v>43</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="I12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>